<commit_message>
fix: Update schema v1.12
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.12.xlsx
+++ b/schema_definitions/template_schema_v1.12.xlsx
@@ -5,25 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karatugo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karatugo/Documents/GitHub/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{9BE1043F-B11B-9342-B852-A3116D29D81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5571E822-6332-2D4D-B7E3-6BAD174E2794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId2"/>
-    <sheet name="association" sheetId="2" r:id="rId3"/>
-    <sheet name="sample" sheetId="3" r:id="rId4"/>
-    <sheet name="notes" sheetId="4" r:id="rId5"/>
+    <sheet name="association" sheetId="2" r:id="rId2"/>
+    <sheet name="sample" sheetId="3" r:id="rId3"/>
+    <sheet name="notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">association!$C$1:$C$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">association!$C$1:$C$15</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1179,7 +1177,7 @@
   </sheetPr>
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
@@ -2598,25 +2596,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD849D0-1EB9-6C46-8E10-56C961C13F81}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3309,7 +3295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -6873,7 +6859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>